<commit_message>
Update with quick lock codes
</commit_message>
<xml_diff>
--- a/ConstructionManual/PartsList.xlsx
+++ b/ConstructionManual/PartsList.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ERSKINA\Repos\AutonoMouseDataSets\FiguresCode\Figures\LesionStudy\ConstructionManual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ERSKINA\Repos\autonomouse-design\ConstructionManual\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Main Frame" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="130">
   <si>
     <t>Item Name</t>
   </si>
@@ -405,6 +405,21 @@
   </si>
   <si>
     <t>Subbase adapter</t>
+  </si>
+  <si>
+    <t>Quick Lock (E slot)</t>
+  </si>
+  <si>
+    <t>1.32.4F2M4.25</t>
+  </si>
+  <si>
+    <t>Quick Lock (Bolt)</t>
+  </si>
+  <si>
+    <t>1.64.5419</t>
+  </si>
+  <si>
+    <t>For different panel thicknesses use different Hmax value. Hmax should be &gt; panel thickness</t>
   </si>
 </sst>
 </file>
@@ -1413,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,45 +1988,76 @@
         <v>94</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+    </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>127</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>97</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
         <v>98</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>